<commit_message>
Mac: Continue with BE correction for multi sample
</commit_message>
<xml_diff>
--- a/DATA/UKSAF/Pt4f.xlsx
+++ b/DATA/UKSAF/Pt4f.xlsx
@@ -8,8 +8,9 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pt4f" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Experimental description" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results Table" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ti2p" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Experimental description" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results Table" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -123,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -148,6 +149,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10027,6 +10031,3841 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D272"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="13" t="inlineStr">
+        <is>
+          <t>BE</t>
+        </is>
+      </c>
+      <c r="B1" s="13" t="inlineStr">
+        <is>
+          <t>Raw Data</t>
+        </is>
+      </c>
+      <c r="C1" s="13" t="inlineStr">
+        <is>
+          <t>Background</t>
+        </is>
+      </c>
+      <c r="D1" s="13" t="inlineStr">
+        <is>
+          <t>Transmission</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>475.08</v>
+      </c>
+      <c r="B2" t="n">
+        <v>39754.6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>39754.6</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>474.98</v>
+      </c>
+      <c r="B3" t="n">
+        <v>39971.8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>39971.8</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>474.88</v>
+      </c>
+      <c r="B4" t="n">
+        <v>39341.5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>39341.5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>474.78</v>
+      </c>
+      <c r="B5" t="n">
+        <v>39615.2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>39615.2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>474.68</v>
+      </c>
+      <c r="B6" t="n">
+        <v>40459.1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>40459.1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>474.58</v>
+      </c>
+      <c r="B7" t="n">
+        <v>40072.4</v>
+      </c>
+      <c r="C7" t="n">
+        <v>40072.4</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>474.48</v>
+      </c>
+      <c r="B8" t="n">
+        <v>39748.3</v>
+      </c>
+      <c r="C8" t="n">
+        <v>39748.3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>474.38</v>
+      </c>
+      <c r="B9" t="n">
+        <v>39559.5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>39559.5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>474.28</v>
+      </c>
+      <c r="B10" t="n">
+        <v>39920.2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>39920.2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>474.18</v>
+      </c>
+      <c r="B11" t="n">
+        <v>39662</v>
+      </c>
+      <c r="C11" t="n">
+        <v>39662</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>474.08</v>
+      </c>
+      <c r="B12" t="n">
+        <v>40092</v>
+      </c>
+      <c r="C12" t="n">
+        <v>40092</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>473.98</v>
+      </c>
+      <c r="B13" t="n">
+        <v>40064.8</v>
+      </c>
+      <c r="C13" t="n">
+        <v>40064.8</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>473.88</v>
+      </c>
+      <c r="B14" t="n">
+        <v>39726.5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>39726.5</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>473.78</v>
+      </c>
+      <c r="B15" t="n">
+        <v>40747.4</v>
+      </c>
+      <c r="C15" t="n">
+        <v>40747.4</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>473.68</v>
+      </c>
+      <c r="B16" t="n">
+        <v>41280.5</v>
+      </c>
+      <c r="C16" t="n">
+        <v>41280.5</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>473.58</v>
+      </c>
+      <c r="B17" t="n">
+        <v>40728.5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>40728.5</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>473.48</v>
+      </c>
+      <c r="B18" t="n">
+        <v>41425.5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>41425.5</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>473.38</v>
+      </c>
+      <c r="B19" t="n">
+        <v>41429.8</v>
+      </c>
+      <c r="C19" t="n">
+        <v>41429.8</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>473.28</v>
+      </c>
+      <c r="B20" t="n">
+        <v>41728.1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>41728.1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>473.18</v>
+      </c>
+      <c r="B21" t="n">
+        <v>41685.1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>41685.1</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>473.08</v>
+      </c>
+      <c r="B22" t="n">
+        <v>41736.7</v>
+      </c>
+      <c r="C22" t="n">
+        <v>41736.7</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>472.98</v>
+      </c>
+      <c r="B23" t="n">
+        <v>42194.9</v>
+      </c>
+      <c r="C23" t="n">
+        <v>42194.9</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>472.88</v>
+      </c>
+      <c r="B24" t="n">
+        <v>42707.3</v>
+      </c>
+      <c r="C24" t="n">
+        <v>42707.3</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>472.78</v>
+      </c>
+      <c r="B25" t="n">
+        <v>42958.4</v>
+      </c>
+      <c r="C25" t="n">
+        <v>42958.4</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>472.68</v>
+      </c>
+      <c r="B26" t="n">
+        <v>42753.2</v>
+      </c>
+      <c r="C26" t="n">
+        <v>42753.2</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>472.58</v>
+      </c>
+      <c r="B27" t="n">
+        <v>43503</v>
+      </c>
+      <c r="C27" t="n">
+        <v>43503</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>472.48</v>
+      </c>
+      <c r="B28" t="n">
+        <v>43487.1</v>
+      </c>
+      <c r="C28" t="n">
+        <v>43487.1</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>472.38</v>
+      </c>
+      <c r="B29" t="n">
+        <v>43224.6</v>
+      </c>
+      <c r="C29" t="n">
+        <v>43224.6</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>472.28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>43880.6</v>
+      </c>
+      <c r="C30" t="n">
+        <v>43880.6</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>472.18</v>
+      </c>
+      <c r="B31" t="n">
+        <v>43020.9</v>
+      </c>
+      <c r="C31" t="n">
+        <v>43020.9</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>472.08</v>
+      </c>
+      <c r="B32" t="n">
+        <v>43735.4</v>
+      </c>
+      <c r="C32" t="n">
+        <v>43735.4</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>471.98</v>
+      </c>
+      <c r="B33" t="n">
+        <v>43776.9</v>
+      </c>
+      <c r="C33" t="n">
+        <v>43776.9</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>471.88</v>
+      </c>
+      <c r="B34" t="n">
+        <v>43034.5</v>
+      </c>
+      <c r="C34" t="n">
+        <v>43034.5</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>471.78</v>
+      </c>
+      <c r="B35" t="n">
+        <v>44211.1</v>
+      </c>
+      <c r="C35" t="n">
+        <v>44211.1</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>471.68</v>
+      </c>
+      <c r="B36" t="n">
+        <v>43680.1</v>
+      </c>
+      <c r="C36" t="n">
+        <v>43680.1</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>471.58</v>
+      </c>
+      <c r="B37" t="n">
+        <v>42857.2</v>
+      </c>
+      <c r="C37" t="n">
+        <v>42857.2</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>471.48</v>
+      </c>
+      <c r="B38" t="n">
+        <v>42952.2</v>
+      </c>
+      <c r="C38" t="n">
+        <v>42952.2</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>471.38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>43123.5</v>
+      </c>
+      <c r="C39" t="n">
+        <v>43123.5</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>471.28</v>
+      </c>
+      <c r="B40" t="n">
+        <v>43073.8</v>
+      </c>
+      <c r="C40" t="n">
+        <v>43073.8</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>471.18</v>
+      </c>
+      <c r="B41" t="n">
+        <v>43506</v>
+      </c>
+      <c r="C41" t="n">
+        <v>43506</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>471.08</v>
+      </c>
+      <c r="B42" t="n">
+        <v>43038.8</v>
+      </c>
+      <c r="C42" t="n">
+        <v>43038.8</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>470.98</v>
+      </c>
+      <c r="B43" t="n">
+        <v>42615.4</v>
+      </c>
+      <c r="C43" t="n">
+        <v>42615.4</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>470.88</v>
+      </c>
+      <c r="B44" t="n">
+        <v>42516.5</v>
+      </c>
+      <c r="C44" t="n">
+        <v>42516.5</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>470.78</v>
+      </c>
+      <c r="B45" t="n">
+        <v>42618.4</v>
+      </c>
+      <c r="C45" t="n">
+        <v>42618.4</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>470.68</v>
+      </c>
+      <c r="B46" t="n">
+        <v>42022.7</v>
+      </c>
+      <c r="C46" t="n">
+        <v>42022.7</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>470.58</v>
+      </c>
+      <c r="B47" t="n">
+        <v>41575.6</v>
+      </c>
+      <c r="C47" t="n">
+        <v>41575.6</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>470.48</v>
+      </c>
+      <c r="B48" t="n">
+        <v>41282.9</v>
+      </c>
+      <c r="C48" t="n">
+        <v>41282.9</v>
+      </c>
+      <c r="D48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>470.38</v>
+      </c>
+      <c r="B49" t="n">
+        <v>41105.6</v>
+      </c>
+      <c r="C49" t="n">
+        <v>41105.6</v>
+      </c>
+      <c r="D49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>470.28</v>
+      </c>
+      <c r="B50" t="n">
+        <v>40732.2</v>
+      </c>
+      <c r="C50" t="n">
+        <v>40732.2</v>
+      </c>
+      <c r="D50" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>470.18</v>
+      </c>
+      <c r="B51" t="n">
+        <v>40497.5</v>
+      </c>
+      <c r="C51" t="n">
+        <v>40497.5</v>
+      </c>
+      <c r="D51" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>470.08</v>
+      </c>
+      <c r="B52" t="n">
+        <v>40692.9</v>
+      </c>
+      <c r="C52" t="n">
+        <v>40692.9</v>
+      </c>
+      <c r="D52" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>469.98</v>
+      </c>
+      <c r="B53" t="n">
+        <v>40088.3</v>
+      </c>
+      <c r="C53" t="n">
+        <v>40088.3</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>469.88</v>
+      </c>
+      <c r="B54" t="n">
+        <v>40540.7</v>
+      </c>
+      <c r="C54" t="n">
+        <v>40540.7</v>
+      </c>
+      <c r="D54" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>469.78</v>
+      </c>
+      <c r="B55" t="n">
+        <v>40112</v>
+      </c>
+      <c r="C55" t="n">
+        <v>40112</v>
+      </c>
+      <c r="D55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>469.68</v>
+      </c>
+      <c r="B56" t="n">
+        <v>39632.5</v>
+      </c>
+      <c r="C56" t="n">
+        <v>39632.5</v>
+      </c>
+      <c r="D56" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>469.58</v>
+      </c>
+      <c r="B57" t="n">
+        <v>39119.8</v>
+      </c>
+      <c r="C57" t="n">
+        <v>39119.8</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>469.48</v>
+      </c>
+      <c r="B58" t="n">
+        <v>39416.4</v>
+      </c>
+      <c r="C58" t="n">
+        <v>39416.4</v>
+      </c>
+      <c r="D58" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>469.38</v>
+      </c>
+      <c r="B59" t="n">
+        <v>39218</v>
+      </c>
+      <c r="C59" t="n">
+        <v>39218</v>
+      </c>
+      <c r="D59" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>469.28</v>
+      </c>
+      <c r="B60" t="n">
+        <v>39187.2</v>
+      </c>
+      <c r="C60" t="n">
+        <v>39187.2</v>
+      </c>
+      <c r="D60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>469.18</v>
+      </c>
+      <c r="B61" t="n">
+        <v>38351.3</v>
+      </c>
+      <c r="C61" t="n">
+        <v>38351.3</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>469.08</v>
+      </c>
+      <c r="B62" t="n">
+        <v>38289.6</v>
+      </c>
+      <c r="C62" t="n">
+        <v>38289.6</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>468.98</v>
+      </c>
+      <c r="B63" t="n">
+        <v>37882.1</v>
+      </c>
+      <c r="C63" t="n">
+        <v>37882.1</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>468.88</v>
+      </c>
+      <c r="B64" t="n">
+        <v>38425.6</v>
+      </c>
+      <c r="C64" t="n">
+        <v>38425.6</v>
+      </c>
+      <c r="D64" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>468.78</v>
+      </c>
+      <c r="B65" t="n">
+        <v>38451</v>
+      </c>
+      <c r="C65" t="n">
+        <v>38451</v>
+      </c>
+      <c r="D65" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>468.68</v>
+      </c>
+      <c r="B66" t="n">
+        <v>37652.8</v>
+      </c>
+      <c r="C66" t="n">
+        <v>37652.8</v>
+      </c>
+      <c r="D66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>468.58</v>
+      </c>
+      <c r="B67" t="n">
+        <v>37679.5</v>
+      </c>
+      <c r="C67" t="n">
+        <v>37679.5</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>468.48</v>
+      </c>
+      <c r="B68" t="n">
+        <v>36974.1</v>
+      </c>
+      <c r="C68" t="n">
+        <v>36974.1</v>
+      </c>
+      <c r="D68" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>468.38</v>
+      </c>
+      <c r="B69" t="n">
+        <v>36456.5</v>
+      </c>
+      <c r="C69" t="n">
+        <v>36456.5</v>
+      </c>
+      <c r="D69" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>468.28</v>
+      </c>
+      <c r="B70" t="n">
+        <v>36153.1</v>
+      </c>
+      <c r="C70" t="n">
+        <v>36153.1</v>
+      </c>
+      <c r="D70" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>468.18</v>
+      </c>
+      <c r="B71" t="n">
+        <v>36563.3</v>
+      </c>
+      <c r="C71" t="n">
+        <v>36563.3</v>
+      </c>
+      <c r="D71" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>468.08</v>
+      </c>
+      <c r="B72" t="n">
+        <v>36024.3</v>
+      </c>
+      <c r="C72" t="n">
+        <v>36024.3</v>
+      </c>
+      <c r="D72" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>467.98</v>
+      </c>
+      <c r="B73" t="n">
+        <v>36762</v>
+      </c>
+      <c r="C73" t="n">
+        <v>36762</v>
+      </c>
+      <c r="D73" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>467.88</v>
+      </c>
+      <c r="B74" t="n">
+        <v>36482.3</v>
+      </c>
+      <c r="C74" t="n">
+        <v>36482.3</v>
+      </c>
+      <c r="D74" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>467.78</v>
+      </c>
+      <c r="B75" t="n">
+        <v>35682.1</v>
+      </c>
+      <c r="C75" t="n">
+        <v>35682.1</v>
+      </c>
+      <c r="D75" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>467.68</v>
+      </c>
+      <c r="B76" t="n">
+        <v>36001.6</v>
+      </c>
+      <c r="C76" t="n">
+        <v>36001.6</v>
+      </c>
+      <c r="D76" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>467.58</v>
+      </c>
+      <c r="B77" t="n">
+        <v>35875.7</v>
+      </c>
+      <c r="C77" t="n">
+        <v>35875.7</v>
+      </c>
+      <c r="D77" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>467.48</v>
+      </c>
+      <c r="B78" t="n">
+        <v>36327.1</v>
+      </c>
+      <c r="C78" t="n">
+        <v>36327.1</v>
+      </c>
+      <c r="D78" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>467.38</v>
+      </c>
+      <c r="B79" t="n">
+        <v>35330.9</v>
+      </c>
+      <c r="C79" t="n">
+        <v>35330.9</v>
+      </c>
+      <c r="D79" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>467.28</v>
+      </c>
+      <c r="B80" t="n">
+        <v>36305.9</v>
+      </c>
+      <c r="C80" t="n">
+        <v>35911.4</v>
+      </c>
+      <c r="D80" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>467.18</v>
+      </c>
+      <c r="B81" t="n">
+        <v>35775.8</v>
+      </c>
+      <c r="C81" t="n">
+        <v>35837.09</v>
+      </c>
+      <c r="D81" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>467.08</v>
+      </c>
+      <c r="B82" t="n">
+        <v>35652.5</v>
+      </c>
+      <c r="C82" t="n">
+        <v>35836.59</v>
+      </c>
+      <c r="D82" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>466.98</v>
+      </c>
+      <c r="B83" t="n">
+        <v>35385.4</v>
+      </c>
+      <c r="C83" t="n">
+        <v>35836.98</v>
+      </c>
+      <c r="D83" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>466.88</v>
+      </c>
+      <c r="B84" t="n">
+        <v>36313</v>
+      </c>
+      <c r="C84" t="n">
+        <v>35837.94</v>
+      </c>
+      <c r="D84" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>466.78</v>
+      </c>
+      <c r="B85" t="n">
+        <v>36285.8</v>
+      </c>
+      <c r="C85" t="n">
+        <v>35837.89</v>
+      </c>
+      <c r="D85" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>466.68</v>
+      </c>
+      <c r="B86" t="n">
+        <v>36279.6</v>
+      </c>
+      <c r="C86" t="n">
+        <v>35836.47</v>
+      </c>
+      <c r="D86" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>466.58</v>
+      </c>
+      <c r="B87" t="n">
+        <v>36632.5</v>
+      </c>
+      <c r="C87" t="n">
+        <v>35835.09</v>
+      </c>
+      <c r="D87" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>466.48</v>
+      </c>
+      <c r="B88" t="n">
+        <v>37237.3</v>
+      </c>
+      <c r="C88" t="n">
+        <v>35833.16</v>
+      </c>
+      <c r="D88" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>466.38</v>
+      </c>
+      <c r="B89" t="n">
+        <v>37359.8</v>
+      </c>
+      <c r="C89" t="n">
+        <v>35829.75</v>
+      </c>
+      <c r="D89" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>466.28</v>
+      </c>
+      <c r="B90" t="n">
+        <v>38475.3</v>
+      </c>
+      <c r="C90" t="n">
+        <v>35825.2</v>
+      </c>
+      <c r="D90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>466.18</v>
+      </c>
+      <c r="B91" t="n">
+        <v>37899.7</v>
+      </c>
+      <c r="C91" t="n">
+        <v>35818.75</v>
+      </c>
+      <c r="D91" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>466.08</v>
+      </c>
+      <c r="B92" t="n">
+        <v>37570.5</v>
+      </c>
+      <c r="C92" t="n">
+        <v>35811.48</v>
+      </c>
+      <c r="D92" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>465.98</v>
+      </c>
+      <c r="B93" t="n">
+        <v>38412.2</v>
+      </c>
+      <c r="C93" t="n">
+        <v>35805.55</v>
+      </c>
+      <c r="D93" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>465.88</v>
+      </c>
+      <c r="B94" t="n">
+        <v>38787</v>
+      </c>
+      <c r="C94" t="n">
+        <v>35798.78</v>
+      </c>
+      <c r="D94" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>465.78</v>
+      </c>
+      <c r="B95" t="n">
+        <v>39270.7</v>
+      </c>
+      <c r="C95" t="n">
+        <v>35790.13</v>
+      </c>
+      <c r="D95" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>465.68</v>
+      </c>
+      <c r="B96" t="n">
+        <v>39573.3</v>
+      </c>
+      <c r="C96" t="n">
+        <v>35780.13</v>
+      </c>
+      <c r="D96" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>465.58</v>
+      </c>
+      <c r="B97" t="n">
+        <v>40278.3</v>
+      </c>
+      <c r="C97" t="n">
+        <v>35768.87</v>
+      </c>
+      <c r="D97" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>465.48</v>
+      </c>
+      <c r="B98" t="n">
+        <v>40182.2</v>
+      </c>
+      <c r="C98" t="n">
+        <v>35756.03</v>
+      </c>
+      <c r="D98" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>465.38</v>
+      </c>
+      <c r="B99" t="n">
+        <v>40908.6</v>
+      </c>
+      <c r="C99" t="n">
+        <v>35742.22</v>
+      </c>
+      <c r="D99" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>465.28</v>
+      </c>
+      <c r="B100" t="n">
+        <v>41359.4</v>
+      </c>
+      <c r="C100" t="n">
+        <v>35727.35</v>
+      </c>
+      <c r="D100" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>465.18</v>
+      </c>
+      <c r="B101" t="n">
+        <v>42018.6</v>
+      </c>
+      <c r="C101" t="n">
+        <v>35710.62</v>
+      </c>
+      <c r="D101" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>465.08</v>
+      </c>
+      <c r="B102" t="n">
+        <v>43477.4</v>
+      </c>
+      <c r="C102" t="n">
+        <v>35692.04</v>
+      </c>
+      <c r="D102" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>464.98</v>
+      </c>
+      <c r="B103" t="n">
+        <v>44431.8</v>
+      </c>
+      <c r="C103" t="n">
+        <v>35670.1</v>
+      </c>
+      <c r="D103" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>464.88</v>
+      </c>
+      <c r="B104" t="n">
+        <v>45237.4</v>
+      </c>
+      <c r="C104" t="n">
+        <v>35644.37</v>
+      </c>
+      <c r="D104" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>464.78</v>
+      </c>
+      <c r="B105" t="n">
+        <v>46298.1</v>
+      </c>
+      <c r="C105" t="n">
+        <v>35615.82</v>
+      </c>
+      <c r="D105" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>464.68</v>
+      </c>
+      <c r="B106" t="n">
+        <v>48371.8</v>
+      </c>
+      <c r="C106" t="n">
+        <v>35584.13</v>
+      </c>
+      <c r="D106" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>464.58</v>
+      </c>
+      <c r="B107" t="n">
+        <v>49874.7</v>
+      </c>
+      <c r="C107" t="n">
+        <v>35547.38</v>
+      </c>
+      <c r="D107" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>464.48</v>
+      </c>
+      <c r="B108" t="n">
+        <v>52045.5</v>
+      </c>
+      <c r="C108" t="n">
+        <v>35504.89</v>
+      </c>
+      <c r="D108" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>464.38</v>
+      </c>
+      <c r="B109" t="n">
+        <v>53500.1</v>
+      </c>
+      <c r="C109" t="n">
+        <v>35456.47</v>
+      </c>
+      <c r="D109" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>464.28</v>
+      </c>
+      <c r="B110" t="n">
+        <v>56491.5</v>
+      </c>
+      <c r="C110" t="n">
+        <v>35402.04</v>
+      </c>
+      <c r="D110" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>464.18</v>
+      </c>
+      <c r="B111" t="n">
+        <v>58241.6</v>
+      </c>
+      <c r="C111" t="n">
+        <v>35340.32</v>
+      </c>
+      <c r="D111" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>464.08</v>
+      </c>
+      <c r="B112" t="n">
+        <v>58492.2</v>
+      </c>
+      <c r="C112" t="n">
+        <v>35271.36</v>
+      </c>
+      <c r="D112" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>463.98</v>
+      </c>
+      <c r="B113" t="n">
+        <v>59993.4</v>
+      </c>
+      <c r="C113" t="n">
+        <v>35199.04</v>
+      </c>
+      <c r="D113" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>463.88</v>
+      </c>
+      <c r="B114" t="n">
+        <v>60943.2</v>
+      </c>
+      <c r="C114" t="n">
+        <v>35123.52</v>
+      </c>
+      <c r="D114" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>463.78</v>
+      </c>
+      <c r="B115" t="n">
+        <v>60757.5</v>
+      </c>
+      <c r="C115" t="n">
+        <v>35044.25</v>
+      </c>
+      <c r="D115" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>463.68</v>
+      </c>
+      <c r="B116" t="n">
+        <v>61064.9</v>
+      </c>
+      <c r="C116" t="n">
+        <v>34963.67</v>
+      </c>
+      <c r="D116" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>463.58</v>
+      </c>
+      <c r="B117" t="n">
+        <v>60081.4</v>
+      </c>
+      <c r="C117" t="n">
+        <v>34882.89</v>
+      </c>
+      <c r="D117" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>463.48</v>
+      </c>
+      <c r="B118" t="n">
+        <v>58455.2</v>
+      </c>
+      <c r="C118" t="n">
+        <v>34803.56</v>
+      </c>
+      <c r="D118" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>463.38</v>
+      </c>
+      <c r="B119" t="n">
+        <v>57070.7</v>
+      </c>
+      <c r="C119" t="n">
+        <v>34728.31</v>
+      </c>
+      <c r="D119" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>463.28</v>
+      </c>
+      <c r="B120" t="n">
+        <v>54895.6</v>
+      </c>
+      <c r="C120" t="n">
+        <v>34657.83</v>
+      </c>
+      <c r="D120" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>463.18</v>
+      </c>
+      <c r="B121" t="n">
+        <v>53543.9</v>
+      </c>
+      <c r="C121" t="n">
+        <v>34592.81</v>
+      </c>
+      <c r="D121" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>463.08</v>
+      </c>
+      <c r="B122" t="n">
+        <v>52083.7</v>
+      </c>
+      <c r="C122" t="n">
+        <v>34532.9</v>
+      </c>
+      <c r="D122" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>462.98</v>
+      </c>
+      <c r="B123" t="n">
+        <v>50127</v>
+      </c>
+      <c r="C123" t="n">
+        <v>34477.52</v>
+      </c>
+      <c r="D123" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>462.88</v>
+      </c>
+      <c r="B124" t="n">
+        <v>48588.1</v>
+      </c>
+      <c r="C124" t="n">
+        <v>34427.4</v>
+      </c>
+      <c r="D124" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>462.78</v>
+      </c>
+      <c r="B125" t="n">
+        <v>47326.9</v>
+      </c>
+      <c r="C125" t="n">
+        <v>34382.34</v>
+      </c>
+      <c r="D125" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>462.68</v>
+      </c>
+      <c r="B126" t="n">
+        <v>46217.6</v>
+      </c>
+      <c r="C126" t="n">
+        <v>34341.35</v>
+      </c>
+      <c r="D126" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>462.58</v>
+      </c>
+      <c r="B127" t="n">
+        <v>45448.5</v>
+      </c>
+      <c r="C127" t="n">
+        <v>34303.72</v>
+      </c>
+      <c r="D127" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>462.48</v>
+      </c>
+      <c r="B128" t="n">
+        <v>44004.5</v>
+      </c>
+      <c r="C128" t="n">
+        <v>34269.08</v>
+      </c>
+      <c r="D128" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>462.38</v>
+      </c>
+      <c r="B129" t="n">
+        <v>42300.8</v>
+      </c>
+      <c r="C129" t="n">
+        <v>34238.26</v>
+      </c>
+      <c r="D129" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>462.28</v>
+      </c>
+      <c r="B130" t="n">
+        <v>41976.4</v>
+      </c>
+      <c r="C130" t="n">
+        <v>34211.7</v>
+      </c>
+      <c r="D130" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>462.18</v>
+      </c>
+      <c r="B131" t="n">
+        <v>40976</v>
+      </c>
+      <c r="C131" t="n">
+        <v>34187.87</v>
+      </c>
+      <c r="D131" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>462.08</v>
+      </c>
+      <c r="B132" t="n">
+        <v>39662.7</v>
+      </c>
+      <c r="C132" t="n">
+        <v>34166.54</v>
+      </c>
+      <c r="D132" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>461.98</v>
+      </c>
+      <c r="B133" t="n">
+        <v>39619.2</v>
+      </c>
+      <c r="C133" t="n">
+        <v>34148.24</v>
+      </c>
+      <c r="D133" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>461.88</v>
+      </c>
+      <c r="B134" t="n">
+        <v>39377.8</v>
+      </c>
+      <c r="C134" t="n">
+        <v>34131.44</v>
+      </c>
+      <c r="D134" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>461.78</v>
+      </c>
+      <c r="B135" t="n">
+        <v>38388.1</v>
+      </c>
+      <c r="C135" t="n">
+        <v>34115.52</v>
+      </c>
+      <c r="D135" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>461.68</v>
+      </c>
+      <c r="B136" t="n">
+        <v>38223</v>
+      </c>
+      <c r="C136" t="n">
+        <v>34101.42</v>
+      </c>
+      <c r="D136" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>461.58</v>
+      </c>
+      <c r="B137" t="n">
+        <v>36865.2</v>
+      </c>
+      <c r="C137" t="n">
+        <v>34089.26</v>
+      </c>
+      <c r="D137" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>461.48</v>
+      </c>
+      <c r="B138" t="n">
+        <v>36879.5</v>
+      </c>
+      <c r="C138" t="n">
+        <v>34079.33</v>
+      </c>
+      <c r="D138" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>461.38</v>
+      </c>
+      <c r="B139" t="n">
+        <v>36851.5</v>
+      </c>
+      <c r="C139" t="n">
+        <v>34070.73</v>
+      </c>
+      <c r="D139" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>461.28</v>
+      </c>
+      <c r="B140" t="n">
+        <v>36886.4</v>
+      </c>
+      <c r="C140" t="n">
+        <v>34062.12</v>
+      </c>
+      <c r="D140" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>461.18</v>
+      </c>
+      <c r="B141" t="n">
+        <v>36040.2</v>
+      </c>
+      <c r="C141" t="n">
+        <v>34053.91</v>
+      </c>
+      <c r="D141" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>461.08</v>
+      </c>
+      <c r="B142" t="n">
+        <v>36166.2</v>
+      </c>
+      <c r="C142" t="n">
+        <v>34046.87</v>
+      </c>
+      <c r="D142" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>460.98</v>
+      </c>
+      <c r="B143" t="n">
+        <v>36580.2</v>
+      </c>
+      <c r="C143" t="n">
+        <v>34040.25</v>
+      </c>
+      <c r="D143" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>460.88</v>
+      </c>
+      <c r="B144" t="n">
+        <v>36225.1</v>
+      </c>
+      <c r="C144" t="n">
+        <v>34033.03</v>
+      </c>
+      <c r="D144" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>460.78</v>
+      </c>
+      <c r="B145" t="n">
+        <v>36968.4</v>
+      </c>
+      <c r="C145" t="n">
+        <v>34025.52</v>
+      </c>
+      <c r="D145" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>460.68</v>
+      </c>
+      <c r="B146" t="n">
+        <v>36678</v>
+      </c>
+      <c r="C146" t="n">
+        <v>34017.35</v>
+      </c>
+      <c r="D146" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>460.58</v>
+      </c>
+      <c r="B147" t="n">
+        <v>36365.6</v>
+      </c>
+      <c r="C147" t="n">
+        <v>34009.03</v>
+      </c>
+      <c r="D147" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>460.48</v>
+      </c>
+      <c r="B148" t="n">
+        <v>36258.8</v>
+      </c>
+      <c r="C148" t="n">
+        <v>34001.53</v>
+      </c>
+      <c r="D148" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>460.38</v>
+      </c>
+      <c r="B149" t="n">
+        <v>36255.7</v>
+      </c>
+      <c r="C149" t="n">
+        <v>33994.47</v>
+      </c>
+      <c r="D149" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>460.28</v>
+      </c>
+      <c r="B150" t="n">
+        <v>36053.5</v>
+      </c>
+      <c r="C150" t="n">
+        <v>33987.61</v>
+      </c>
+      <c r="D150" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>460.18</v>
+      </c>
+      <c r="B151" t="n">
+        <v>36402</v>
+      </c>
+      <c r="C151" t="n">
+        <v>33980.86</v>
+      </c>
+      <c r="D151" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>460.08</v>
+      </c>
+      <c r="B152" t="n">
+        <v>37028.1</v>
+      </c>
+      <c r="C152" t="n">
+        <v>33973.39</v>
+      </c>
+      <c r="D152" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>459.98</v>
+      </c>
+      <c r="B153" t="n">
+        <v>37042</v>
+      </c>
+      <c r="C153" t="n">
+        <v>33964.58</v>
+      </c>
+      <c r="D153" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>459.88</v>
+      </c>
+      <c r="B154" t="n">
+        <v>37572.4</v>
+      </c>
+      <c r="C154" t="n">
+        <v>33954.81</v>
+      </c>
+      <c r="D154" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>459.78</v>
+      </c>
+      <c r="B155" t="n">
+        <v>37672.3</v>
+      </c>
+      <c r="C155" t="n">
+        <v>33944.12</v>
+      </c>
+      <c r="D155" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>459.68</v>
+      </c>
+      <c r="B156" t="n">
+        <v>37673</v>
+      </c>
+      <c r="C156" t="n">
+        <v>33932.72</v>
+      </c>
+      <c r="D156" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>459.58</v>
+      </c>
+      <c r="B157" t="n">
+        <v>37782.7</v>
+      </c>
+      <c r="C157" t="n">
+        <v>33921.12</v>
+      </c>
+      <c r="D157" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>459.48</v>
+      </c>
+      <c r="B158" t="n">
+        <v>38926.8</v>
+      </c>
+      <c r="C158" t="n">
+        <v>33908.66</v>
+      </c>
+      <c r="D158" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>459.38</v>
+      </c>
+      <c r="B159" t="n">
+        <v>39739.5</v>
+      </c>
+      <c r="C159" t="n">
+        <v>33893.8</v>
+      </c>
+      <c r="D159" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>459.28</v>
+      </c>
+      <c r="B160" t="n">
+        <v>40351</v>
+      </c>
+      <c r="C160" t="n">
+        <v>33876.17</v>
+      </c>
+      <c r="D160" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>459.18</v>
+      </c>
+      <c r="B161" t="n">
+        <v>41886</v>
+      </c>
+      <c r="C161" t="n">
+        <v>33855.84</v>
+      </c>
+      <c r="D161" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>459.08</v>
+      </c>
+      <c r="B162" t="n">
+        <v>44103.1</v>
+      </c>
+      <c r="C162" t="n">
+        <v>33831.14</v>
+      </c>
+      <c r="D162" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>458.98</v>
+      </c>
+      <c r="B163" t="n">
+        <v>47130.5</v>
+      </c>
+      <c r="C163" t="n">
+        <v>33799.57</v>
+      </c>
+      <c r="D163" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>458.88</v>
+      </c>
+      <c r="B164" t="n">
+        <v>50709.4</v>
+      </c>
+      <c r="C164" t="n">
+        <v>33758.82</v>
+      </c>
+      <c r="D164" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>458.78</v>
+      </c>
+      <c r="B165" t="n">
+        <v>55999.6</v>
+      </c>
+      <c r="C165" t="n">
+        <v>33706.05</v>
+      </c>
+      <c r="D165" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>458.68</v>
+      </c>
+      <c r="B166" t="n">
+        <v>62969.8</v>
+      </c>
+      <c r="C166" t="n">
+        <v>33636.73</v>
+      </c>
+      <c r="D166" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>458.58</v>
+      </c>
+      <c r="B167" t="n">
+        <v>71303.89999999999</v>
+      </c>
+      <c r="C167" t="n">
+        <v>33545.35</v>
+      </c>
+      <c r="D167" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>458.48</v>
+      </c>
+      <c r="B168" t="n">
+        <v>81636.39999999999</v>
+      </c>
+      <c r="C168" t="n">
+        <v>33426.25</v>
+      </c>
+      <c r="D168" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>458.38</v>
+      </c>
+      <c r="B169" t="n">
+        <v>92709.10000000001</v>
+      </c>
+      <c r="C169" t="n">
+        <v>33273.65</v>
+      </c>
+      <c r="D169" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>458.28</v>
+      </c>
+      <c r="B170" t="n">
+        <v>103772</v>
+      </c>
+      <c r="C170" t="n">
+        <v>33083.73</v>
+      </c>
+      <c r="D170" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>458.18</v>
+      </c>
+      <c r="B171" t="n">
+        <v>113444</v>
+      </c>
+      <c r="C171" t="n">
+        <v>32856.27</v>
+      </c>
+      <c r="D171" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>458.08</v>
+      </c>
+      <c r="B172" t="n">
+        <v>119024</v>
+      </c>
+      <c r="C172" t="n">
+        <v>32597.08</v>
+      </c>
+      <c r="D172" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>457.98</v>
+      </c>
+      <c r="B173" t="n">
+        <v>120755</v>
+      </c>
+      <c r="C173" t="n">
+        <v>32318.49</v>
+      </c>
+      <c r="D173" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>457.88</v>
+      </c>
+      <c r="B174" t="n">
+        <v>117239</v>
+      </c>
+      <c r="C174" t="n">
+        <v>32036.54</v>
+      </c>
+      <c r="D174" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>457.78</v>
+      </c>
+      <c r="B175" t="n">
+        <v>108874</v>
+      </c>
+      <c r="C175" t="n">
+        <v>31769.52</v>
+      </c>
+      <c r="D175" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>457.68</v>
+      </c>
+      <c r="B176" t="n">
+        <v>97209</v>
+      </c>
+      <c r="C176" t="n">
+        <v>31533.4</v>
+      </c>
+      <c r="D176" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>457.58</v>
+      </c>
+      <c r="B177" t="n">
+        <v>86220.5</v>
+      </c>
+      <c r="C177" t="n">
+        <v>31334.9</v>
+      </c>
+      <c r="D177" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>457.48</v>
+      </c>
+      <c r="B178" t="n">
+        <v>73988.89999999999</v>
+      </c>
+      <c r="C178" t="n">
+        <v>31175.12</v>
+      </c>
+      <c r="D178" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>457.38</v>
+      </c>
+      <c r="B179" t="n">
+        <v>64204.4</v>
+      </c>
+      <c r="C179" t="n">
+        <v>31051.83</v>
+      </c>
+      <c r="D179" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>457.28</v>
+      </c>
+      <c r="B180" t="n">
+        <v>55645.9</v>
+      </c>
+      <c r="C180" t="n">
+        <v>30958.84</v>
+      </c>
+      <c r="D180" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>457.18</v>
+      </c>
+      <c r="B181" t="n">
+        <v>49088.4</v>
+      </c>
+      <c r="C181" t="n">
+        <v>30890.4</v>
+      </c>
+      <c r="D181" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>457.08</v>
+      </c>
+      <c r="B182" t="n">
+        <v>44998.2</v>
+      </c>
+      <c r="C182" t="n">
+        <v>30839.21</v>
+      </c>
+      <c r="D182" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>456.98</v>
+      </c>
+      <c r="B183" t="n">
+        <v>41793.5</v>
+      </c>
+      <c r="C183" t="n">
+        <v>30799.7</v>
+      </c>
+      <c r="D183" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>456.88</v>
+      </c>
+      <c r="B184" t="n">
+        <v>38432.4</v>
+      </c>
+      <c r="C184" t="n">
+        <v>30770.43</v>
+      </c>
+      <c r="D184" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>456.78</v>
+      </c>
+      <c r="B185" t="n">
+        <v>37270.1</v>
+      </c>
+      <c r="C185" t="n">
+        <v>30748.28</v>
+      </c>
+      <c r="D185" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>456.68</v>
+      </c>
+      <c r="B186" t="n">
+        <v>36334.8</v>
+      </c>
+      <c r="C186" t="n">
+        <v>30729.46</v>
+      </c>
+      <c r="D186" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>456.58</v>
+      </c>
+      <c r="B187" t="n">
+        <v>34625.6</v>
+      </c>
+      <c r="C187" t="n">
+        <v>30714.67</v>
+      </c>
+      <c r="D187" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>456.48</v>
+      </c>
+      <c r="B188" t="n">
+        <v>34150.6</v>
+      </c>
+      <c r="C188" t="n">
+        <v>30703.24</v>
+      </c>
+      <c r="D188" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>456.38</v>
+      </c>
+      <c r="B189" t="n">
+        <v>33500.5</v>
+      </c>
+      <c r="C189" t="n">
+        <v>30693.56</v>
+      </c>
+      <c r="D189" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>456.28</v>
+      </c>
+      <c r="B190" t="n">
+        <v>32882.3</v>
+      </c>
+      <c r="C190" t="n">
+        <v>30685.81</v>
+      </c>
+      <c r="D190" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>456.18</v>
+      </c>
+      <c r="B191" t="n">
+        <v>32781.7</v>
+      </c>
+      <c r="C191" t="n">
+        <v>30679.17</v>
+      </c>
+      <c r="D191" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>456.08</v>
+      </c>
+      <c r="B192" t="n">
+        <v>31582.9</v>
+      </c>
+      <c r="C192" t="n">
+        <v>30674.5</v>
+      </c>
+      <c r="D192" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>455.98</v>
+      </c>
+      <c r="B193" t="n">
+        <v>32062.6</v>
+      </c>
+      <c r="C193" t="n">
+        <v>30670.94</v>
+      </c>
+      <c r="D193" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>455.88</v>
+      </c>
+      <c r="B194" t="n">
+        <v>32227.9</v>
+      </c>
+      <c r="C194" t="n">
+        <v>30666.41</v>
+      </c>
+      <c r="D194" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>455.78</v>
+      </c>
+      <c r="B195" t="n">
+        <v>31659.9</v>
+      </c>
+      <c r="C195" t="n">
+        <v>30662.46</v>
+      </c>
+      <c r="D195" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>455.68</v>
+      </c>
+      <c r="B196" t="n">
+        <v>31408.9</v>
+      </c>
+      <c r="C196" t="n">
+        <v>30659.75</v>
+      </c>
+      <c r="D196" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>455.58</v>
+      </c>
+      <c r="B197" t="n">
+        <v>31413.7</v>
+      </c>
+      <c r="C197" t="n">
+        <v>30657.43</v>
+      </c>
+      <c r="D197" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>455.48</v>
+      </c>
+      <c r="B198" t="n">
+        <v>31525.9</v>
+      </c>
+      <c r="C198" t="n">
+        <v>30654.93</v>
+      </c>
+      <c r="D198" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>455.38</v>
+      </c>
+      <c r="B199" t="n">
+        <v>30839.3</v>
+      </c>
+      <c r="C199" t="n">
+        <v>30653.29</v>
+      </c>
+      <c r="D199" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>455.28</v>
+      </c>
+      <c r="B200" t="n">
+        <v>31315</v>
+      </c>
+      <c r="C200" t="n">
+        <v>30651.98</v>
+      </c>
+      <c r="D200" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>455.18</v>
+      </c>
+      <c r="B201" t="n">
+        <v>30985.2</v>
+      </c>
+      <c r="C201" t="n">
+        <v>30650.44</v>
+      </c>
+      <c r="D201" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>455.08</v>
+      </c>
+      <c r="B202" t="n">
+        <v>30875.4</v>
+      </c>
+      <c r="C202" t="n">
+        <v>30649.57</v>
+      </c>
+      <c r="D202" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>454.98</v>
+      </c>
+      <c r="B203" t="n">
+        <v>30713.9</v>
+      </c>
+      <c r="C203" t="n">
+        <v>30649.12</v>
+      </c>
+      <c r="D203" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>454.88</v>
+      </c>
+      <c r="B204" t="n">
+        <v>30565.6</v>
+      </c>
+      <c r="C204" t="n">
+        <v>30649.15</v>
+      </c>
+      <c r="D204" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>454.78</v>
+      </c>
+      <c r="B205" t="n">
+        <v>30870.9</v>
+      </c>
+      <c r="C205" t="n">
+        <v>30648.94</v>
+      </c>
+      <c r="D205" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>454.68</v>
+      </c>
+      <c r="B206" t="n">
+        <v>31009.2</v>
+      </c>
+      <c r="C206" t="n">
+        <v>30648.05</v>
+      </c>
+      <c r="D206" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>454.58</v>
+      </c>
+      <c r="B207" t="n">
+        <v>31029.9</v>
+      </c>
+      <c r="C207" t="n">
+        <v>30646.9</v>
+      </c>
+      <c r="D207" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>454.48</v>
+      </c>
+      <c r="B208" t="n">
+        <v>30333.4</v>
+      </c>
+      <c r="C208" t="n">
+        <v>30646.78</v>
+      </c>
+      <c r="D208" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>454.38</v>
+      </c>
+      <c r="B209" t="n">
+        <v>30287.4</v>
+      </c>
+      <c r="C209" t="n">
+        <v>30647.81</v>
+      </c>
+      <c r="D209" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>454.28</v>
+      </c>
+      <c r="B210" t="n">
+        <v>30217.2</v>
+      </c>
+      <c r="C210" t="n">
+        <v>30649.03</v>
+      </c>
+      <c r="D210" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>454.18</v>
+      </c>
+      <c r="B211" t="n">
+        <v>30891.8</v>
+      </c>
+      <c r="C211" t="n">
+        <v>30649.33</v>
+      </c>
+      <c r="D211" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>454.08</v>
+      </c>
+      <c r="B212" t="n">
+        <v>30333.1</v>
+      </c>
+      <c r="C212" t="n">
+        <v>30649.44</v>
+      </c>
+      <c r="D212" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>453.98</v>
+      </c>
+      <c r="B213" t="n">
+        <v>30538.3</v>
+      </c>
+      <c r="C213" t="n">
+        <v>30650.1</v>
+      </c>
+      <c r="D213" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>453.88</v>
+      </c>
+      <c r="B214" t="n">
+        <v>30385.8</v>
+      </c>
+      <c r="C214" t="n">
+        <v>30385.8</v>
+      </c>
+      <c r="D214" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>453.78</v>
+      </c>
+      <c r="B215" t="n">
+        <v>30989.1</v>
+      </c>
+      <c r="C215" t="n">
+        <v>30989.1</v>
+      </c>
+      <c r="D215" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>453.68</v>
+      </c>
+      <c r="B216" t="n">
+        <v>30624.1</v>
+      </c>
+      <c r="C216" t="n">
+        <v>30624.1</v>
+      </c>
+      <c r="D216" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>453.58</v>
+      </c>
+      <c r="B217" t="n">
+        <v>30723.4</v>
+      </c>
+      <c r="C217" t="n">
+        <v>30723.4</v>
+      </c>
+      <c r="D217" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>453.48</v>
+      </c>
+      <c r="B218" t="n">
+        <v>30451.6</v>
+      </c>
+      <c r="C218" t="n">
+        <v>30451.6</v>
+      </c>
+      <c r="D218" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>453.38</v>
+      </c>
+      <c r="B219" t="n">
+        <v>30635.9</v>
+      </c>
+      <c r="C219" t="n">
+        <v>30635.9</v>
+      </c>
+      <c r="D219" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>453.28</v>
+      </c>
+      <c r="B220" t="n">
+        <v>30125.8</v>
+      </c>
+      <c r="C220" t="n">
+        <v>30125.8</v>
+      </c>
+      <c r="D220" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>453.18</v>
+      </c>
+      <c r="B221" t="n">
+        <v>30531</v>
+      </c>
+      <c r="C221" t="n">
+        <v>30531</v>
+      </c>
+      <c r="D221" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>453.08</v>
+      </c>
+      <c r="B222" t="n">
+        <v>30227.4</v>
+      </c>
+      <c r="C222" t="n">
+        <v>30227.4</v>
+      </c>
+      <c r="D222" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>452.98</v>
+      </c>
+      <c r="B223" t="n">
+        <v>30296</v>
+      </c>
+      <c r="C223" t="n">
+        <v>30296</v>
+      </c>
+      <c r="D223" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>452.88</v>
+      </c>
+      <c r="B224" t="n">
+        <v>30264.3</v>
+      </c>
+      <c r="C224" t="n">
+        <v>30264.3</v>
+      </c>
+      <c r="D224" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>452.78</v>
+      </c>
+      <c r="B225" t="n">
+        <v>30284.3</v>
+      </c>
+      <c r="C225" t="n">
+        <v>30284.3</v>
+      </c>
+      <c r="D225" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>452.68</v>
+      </c>
+      <c r="B226" t="n">
+        <v>30439.6</v>
+      </c>
+      <c r="C226" t="n">
+        <v>30439.6</v>
+      </c>
+      <c r="D226" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>452.58</v>
+      </c>
+      <c r="B227" t="n">
+        <v>30214.6</v>
+      </c>
+      <c r="C227" t="n">
+        <v>30214.6</v>
+      </c>
+      <c r="D227" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>452.48</v>
+      </c>
+      <c r="B228" t="n">
+        <v>30825.9</v>
+      </c>
+      <c r="C228" t="n">
+        <v>30825.9</v>
+      </c>
+      <c r="D228" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>452.38</v>
+      </c>
+      <c r="B229" t="n">
+        <v>30212.1</v>
+      </c>
+      <c r="C229" t="n">
+        <v>30212.1</v>
+      </c>
+      <c r="D229" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>452.28</v>
+      </c>
+      <c r="B230" t="n">
+        <v>30610.7</v>
+      </c>
+      <c r="C230" t="n">
+        <v>30610.7</v>
+      </c>
+      <c r="D230" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>452.18</v>
+      </c>
+      <c r="B231" t="n">
+        <v>30346.7</v>
+      </c>
+      <c r="C231" t="n">
+        <v>30346.7</v>
+      </c>
+      <c r="D231" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>452.08</v>
+      </c>
+      <c r="B232" t="n">
+        <v>29739.6</v>
+      </c>
+      <c r="C232" t="n">
+        <v>29739.6</v>
+      </c>
+      <c r="D232" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>451.98</v>
+      </c>
+      <c r="B233" t="n">
+        <v>30374</v>
+      </c>
+      <c r="C233" t="n">
+        <v>30374</v>
+      </c>
+      <c r="D233" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>451.88</v>
+      </c>
+      <c r="B234" t="n">
+        <v>30580.4</v>
+      </c>
+      <c r="C234" t="n">
+        <v>30580.4</v>
+      </c>
+      <c r="D234" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>451.78</v>
+      </c>
+      <c r="B235" t="n">
+        <v>30454.1</v>
+      </c>
+      <c r="C235" t="n">
+        <v>30454.1</v>
+      </c>
+      <c r="D235" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>451.68</v>
+      </c>
+      <c r="B236" t="n">
+        <v>29955.2</v>
+      </c>
+      <c r="C236" t="n">
+        <v>29955.2</v>
+      </c>
+      <c r="D236" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>451.58</v>
+      </c>
+      <c r="B237" t="n">
+        <v>30165.1</v>
+      </c>
+      <c r="C237" t="n">
+        <v>30165.1</v>
+      </c>
+      <c r="D237" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>451.48</v>
+      </c>
+      <c r="B238" t="n">
+        <v>30325.2</v>
+      </c>
+      <c r="C238" t="n">
+        <v>30325.2</v>
+      </c>
+      <c r="D238" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>451.38</v>
+      </c>
+      <c r="B239" t="n">
+        <v>30971.6</v>
+      </c>
+      <c r="C239" t="n">
+        <v>30971.6</v>
+      </c>
+      <c r="D239" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>451.28</v>
+      </c>
+      <c r="B240" t="n">
+        <v>30521.3</v>
+      </c>
+      <c r="C240" t="n">
+        <v>30521.3</v>
+      </c>
+      <c r="D240" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>451.18</v>
+      </c>
+      <c r="B241" t="n">
+        <v>30670.1</v>
+      </c>
+      <c r="C241" t="n">
+        <v>30670.1</v>
+      </c>
+      <c r="D241" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>451.08</v>
+      </c>
+      <c r="B242" t="n">
+        <v>30170.9</v>
+      </c>
+      <c r="C242" t="n">
+        <v>30170.9</v>
+      </c>
+      <c r="D242" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>450.98</v>
+      </c>
+      <c r="B243" t="n">
+        <v>30373.3</v>
+      </c>
+      <c r="C243" t="n">
+        <v>30373.3</v>
+      </c>
+      <c r="D243" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>450.88</v>
+      </c>
+      <c r="B244" t="n">
+        <v>30766</v>
+      </c>
+      <c r="C244" t="n">
+        <v>30766</v>
+      </c>
+      <c r="D244" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>450.78</v>
+      </c>
+      <c r="B245" t="n">
+        <v>30578.8</v>
+      </c>
+      <c r="C245" t="n">
+        <v>30578.8</v>
+      </c>
+      <c r="D245" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>450.68</v>
+      </c>
+      <c r="B246" t="n">
+        <v>29672.6</v>
+      </c>
+      <c r="C246" t="n">
+        <v>29672.6</v>
+      </c>
+      <c r="D246" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>450.58</v>
+      </c>
+      <c r="B247" t="n">
+        <v>30111</v>
+      </c>
+      <c r="C247" t="n">
+        <v>30111</v>
+      </c>
+      <c r="D247" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>450.48</v>
+      </c>
+      <c r="B248" t="n">
+        <v>30286.2</v>
+      </c>
+      <c r="C248" t="n">
+        <v>30286.2</v>
+      </c>
+      <c r="D248" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>450.38</v>
+      </c>
+      <c r="B249" t="n">
+        <v>30475.6</v>
+      </c>
+      <c r="C249" t="n">
+        <v>30475.6</v>
+      </c>
+      <c r="D249" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>450.28</v>
+      </c>
+      <c r="B250" t="n">
+        <v>30163.7</v>
+      </c>
+      <c r="C250" t="n">
+        <v>30163.7</v>
+      </c>
+      <c r="D250" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>450.18</v>
+      </c>
+      <c r="B251" t="n">
+        <v>30019.2</v>
+      </c>
+      <c r="C251" t="n">
+        <v>30019.2</v>
+      </c>
+      <c r="D251" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>450.08</v>
+      </c>
+      <c r="B252" t="n">
+        <v>29831.2</v>
+      </c>
+      <c r="C252" t="n">
+        <v>29831.2</v>
+      </c>
+      <c r="D252" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>449.98</v>
+      </c>
+      <c r="B253" t="n">
+        <v>30011.3</v>
+      </c>
+      <c r="C253" t="n">
+        <v>30011.3</v>
+      </c>
+      <c r="D253" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>449.88</v>
+      </c>
+      <c r="B254" t="n">
+        <v>30570.4</v>
+      </c>
+      <c r="C254" t="n">
+        <v>30570.4</v>
+      </c>
+      <c r="D254" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>449.78</v>
+      </c>
+      <c r="B255" t="n">
+        <v>29994.1</v>
+      </c>
+      <c r="C255" t="n">
+        <v>29994.1</v>
+      </c>
+      <c r="D255" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>449.68</v>
+      </c>
+      <c r="B256" t="n">
+        <v>30867.8</v>
+      </c>
+      <c r="C256" t="n">
+        <v>30867.8</v>
+      </c>
+      <c r="D256" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>449.58</v>
+      </c>
+      <c r="B257" t="n">
+        <v>30532.7</v>
+      </c>
+      <c r="C257" t="n">
+        <v>30532.7</v>
+      </c>
+      <c r="D257" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>449.48</v>
+      </c>
+      <c r="B258" t="n">
+        <v>30713.9</v>
+      </c>
+      <c r="C258" t="n">
+        <v>30713.9</v>
+      </c>
+      <c r="D258" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>449.38</v>
+      </c>
+      <c r="B259" t="n">
+        <v>30454.5</v>
+      </c>
+      <c r="C259" t="n">
+        <v>30454.5</v>
+      </c>
+      <c r="D259" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>449.28</v>
+      </c>
+      <c r="B260" t="n">
+        <v>30068.4</v>
+      </c>
+      <c r="C260" t="n">
+        <v>30068.4</v>
+      </c>
+      <c r="D260" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>449.18</v>
+      </c>
+      <c r="B261" t="n">
+        <v>29912.4</v>
+      </c>
+      <c r="C261" t="n">
+        <v>29912.4</v>
+      </c>
+      <c r="D261" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>449.08</v>
+      </c>
+      <c r="B262" t="n">
+        <v>30174.8</v>
+      </c>
+      <c r="C262" t="n">
+        <v>30174.8</v>
+      </c>
+      <c r="D262" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>448.98</v>
+      </c>
+      <c r="B263" t="n">
+        <v>30120.3</v>
+      </c>
+      <c r="C263" t="n">
+        <v>30120.3</v>
+      </c>
+      <c r="D263" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>448.88</v>
+      </c>
+      <c r="B264" t="n">
+        <v>30110.4</v>
+      </c>
+      <c r="C264" t="n">
+        <v>30110.4</v>
+      </c>
+      <c r="D264" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>448.78</v>
+      </c>
+      <c r="B265" t="n">
+        <v>30306.8</v>
+      </c>
+      <c r="C265" t="n">
+        <v>30306.8</v>
+      </c>
+      <c r="D265" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>448.68</v>
+      </c>
+      <c r="B266" t="n">
+        <v>29977.1</v>
+      </c>
+      <c r="C266" t="n">
+        <v>29977.1</v>
+      </c>
+      <c r="D266" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>448.58</v>
+      </c>
+      <c r="B267" t="n">
+        <v>30408.4</v>
+      </c>
+      <c r="C267" t="n">
+        <v>30408.4</v>
+      </c>
+      <c r="D267" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>448.48</v>
+      </c>
+      <c r="B268" t="n">
+        <v>30672.7</v>
+      </c>
+      <c r="C268" t="n">
+        <v>30672.7</v>
+      </c>
+      <c r="D268" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>448.38</v>
+      </c>
+      <c r="B269" t="n">
+        <v>30340.6</v>
+      </c>
+      <c r="C269" t="n">
+        <v>30340.6</v>
+      </c>
+      <c r="D269" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="n">
+        <v>448.28</v>
+      </c>
+      <c r="B270" t="n">
+        <v>29974.9</v>
+      </c>
+      <c r="C270" t="n">
+        <v>29974.9</v>
+      </c>
+      <c r="D270" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="n">
+        <v>448.18</v>
+      </c>
+      <c r="B271" t="n">
+        <v>30914.7</v>
+      </c>
+      <c r="C271" t="n">
+        <v>30914.7</v>
+      </c>
+      <c r="D271" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>448.08</v>
+      </c>
+      <c r="B272" t="n">
+        <v>30207.3</v>
+      </c>
+      <c r="C272" t="n">
+        <v>30207.3</v>
+      </c>
+      <c r="D272" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10539,13 +14378,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD2"/>
+  <dimension ref="B2:AD2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10585,7 +14424,6 @@
     <col width="14" customWidth="1" min="30" max="30"/>
   </cols>
   <sheetData>
-    <row r="1"/>
     <row r="2">
       <c r="B2" s="12" t="inlineStr">
         <is>

</xml_diff>